<commit_message>
feat(DWIE): update competitons excel for companies
</commit_message>
<xml_diff>
--- a/DWIE/Eval1/Tema2/Tareas/Competencia.xlsx
+++ b/DWIE/Eval1/Tema2/Tareas/Competencia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/576013fc49f8ea2d/Escritorio/IES TEIS/EIE 24-25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a23braisbm\Desktop\daw-notes\DWIE\Eval1\Tema2\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF3F180A-AE68-4C3D-B3F1-B3DC106FED08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126D5B46-F5F3-4393-90BB-667D227EF189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Denominación social</t>
   </si>
@@ -43,22 +43,25 @@
     <t>Otra información</t>
   </si>
   <si>
-    <t>MONCHO Y SANTOME SL</t>
-  </si>
-  <si>
-    <t>CALLE DO HOSPITAL, 7 - BAJO</t>
-  </si>
-  <si>
-    <t>VILALBA</t>
-  </si>
-  <si>
-    <t>https://www.monchoysantome.com/domotica.html</t>
-  </si>
-  <si>
-    <t>Instalación de Domótica y Telecomunicaciones</t>
-  </si>
-  <si>
-    <t>Ver foto adjunta</t>
+    <t>Ro</t>
+  </si>
+  <si>
+    <t>Rover</t>
+  </si>
+  <si>
+    <t>PetCareNow, Inc.</t>
+  </si>
+  <si>
+    <t>EEUU</t>
+  </si>
+  <si>
+    <t>https://www.rover.com/es/</t>
+  </si>
+  <si>
+    <t>Cuidado de mascotas</t>
+  </si>
+  <si>
+    <t>Paseo de mascotas, guardería, visitas a domicilio, hotel, cobertura con seguro</t>
   </si>
 </sst>
 </file>
@@ -151,15 +154,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,9 +198,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4867275" cy="2343150"/>
     <xdr:pic>
@@ -205,6 +221,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12696825" y="352425"/>
+          <a:ext cx="4867275" cy="2343150"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -419,17 +439,19 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="39.08984375" customWidth="1"/>
-    <col min="5" max="5" width="37.90625" customWidth="1"/>
-    <col min="6" max="6" width="27.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" customHeight="1">
@@ -455,29 +477,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="25.5">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="12.75">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="12.5">
-      <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -485,8 +509,8 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="12.5">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:7" ht="12.75">
+      <c r="A4" s="4"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -494,8 +518,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="12.5">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:7" ht="12.75">
+      <c r="A5" s="4"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -503,8 +527,8 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="12.5">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:7" ht="12.75">
+      <c r="A6" s="4"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -512,8 +536,8 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="12.5">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:7" ht="12.75">
+      <c r="A7" s="4"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -521,8 +545,8 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="12.5">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:7" ht="12.75">
+      <c r="A8" s="4"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -530,8 +554,8 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="12.5">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:7" ht="12.75">
+      <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -539,8 +563,8 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="12.5">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:7" ht="12.75">
+      <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -548,8 +572,8 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="12.5">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:7" ht="12.75">
+      <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -557,8 +581,8 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="12.5">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:7" ht="12.75">
+      <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -566,8 +590,8 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="12.5">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:7" ht="12.75">
+      <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -575,8 +599,8 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="12.5">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:7" ht="12.75">
+      <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -584,20 +608,18 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="12.5">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+    <row r="15" spans="1:7" ht="12.75">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>